<commit_message>
integrating wbi tools, common
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\ksp-mod-dev\WBIPlaymodeUSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15C7970-CD66-40A8-970C-C14A837BC6ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFB8B89-C982-4572-9413-272C1047E487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>List of WBI parts and according USI configuration</t>
   </si>
@@ -210,12 +210,6 @@
     <t>60%/2</t>
   </si>
   <si>
-    <t>todo: configure for LS converter option!</t>
-  </si>
-  <si>
-    <t>todo: supplies as storage option</t>
-  </si>
-  <si>
     <t>Bigby Crew Module</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>wip</t>
-  </si>
-  <si>
     <t>m = KerbalMonths (add time directly)</t>
   </si>
   <si>
@@ -247,6 +238,9 @@
   </si>
   <si>
     <t>/n = n kerbal capacity</t>
+  </si>
+  <si>
+    <t>option for LS purifier</t>
   </si>
 </sst>
 </file>
@@ -256,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,13 +308,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -329,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,11 +346,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -374,15 +356,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -404,16 +385,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
-    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
+    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,7 +674,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,19 +697,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J2" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -777,7 +756,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
@@ -818,7 +797,7 @@
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>27</v>
@@ -827,7 +806,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -837,10 +816,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>15</v>
@@ -853,7 +832,7 @@
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>27</v>
@@ -862,7 +841,7 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -890,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>27</v>
@@ -923,7 +902,7 @@
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>27</v>
@@ -957,15 +936,15 @@
       <c r="G9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>69</v>
+      <c r="H9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="14" t="s">
-        <v>61</v>
+      <c r="K9" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -977,7 +956,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -989,14 +968,14 @@
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="14"/>
       <c r="L10" s="10"/>
       <c r="M10" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -1024,7 +1003,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I11" t="s">
         <v>33</v>
@@ -1062,7 +1041,7 @@
         <v>38</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
         <v>58</v>
@@ -1091,7 +1070,7 @@
         <v>41</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
         <v>33</v>
@@ -1123,7 +1102,7 @@
         <v>46</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
         <v>47</v>
@@ -1146,7 +1125,7 @@
         <v>56</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
         <v>55</v>
@@ -1175,7 +1154,7 @@
         <v>0.6875</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
         <v>47</v>
@@ -1206,8 +1185,8 @@
       <c r="G17" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="17" t="s">
-        <v>69</v>
+      <c r="H17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="I17" t="s">
         <v>51</v>
@@ -1215,7 +1194,7 @@
       <c r="K17" t="s">
         <v>60</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="15" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DSEV parts pass #1
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\ksp-mod-dev\WBIPlaymodeUSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A8E47-A31D-4DF4-A3F5-1FB7340CE38E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C385D4-4792-45A3-882E-81A62836270E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="139">
   <si>
     <t>List of WBI parts and according USI configuration</t>
   </si>
@@ -255,9 +255,6 @@
     <t>no additional LS functions</t>
   </si>
   <si>
-    <t>Supplies 50</t>
-  </si>
-  <si>
     <t>WBI_CrewCab</t>
   </si>
   <si>
@@ -292,6 +289,159 @@
   </si>
   <si>
     <t>1m/4</t>
+  </si>
+  <si>
+    <t>DSEV</t>
+  </si>
+  <si>
+    <t>wbiAutomatedConstructionHangar</t>
+  </si>
+  <si>
+    <t>Automated Construction Hangar</t>
+  </si>
+  <si>
+    <t>ELLaunchpad</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>nautilusAirlock</t>
+  </si>
+  <si>
+    <t>Nautilus Airlock</t>
+  </si>
+  <si>
+    <t>wbiNautilusCentrifuge</t>
+  </si>
+  <si>
+    <t>Nautilus Centrifuge</t>
+  </si>
+  <si>
+    <t>Efficiency Part</t>
+  </si>
+  <si>
+    <t>x, tbd</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>WBI_D2Lab</t>
+  </si>
+  <si>
+    <t>D2 Science Module</t>
+  </si>
+  <si>
+    <t>WBIMultipurposeLab:D2LAB;PATH_SCIENCE</t>
+  </si>
+  <si>
+    <t>50%/4</t>
+  </si>
+  <si>
+    <t>WBI_D2Centrifuge</t>
+  </si>
+  <si>
+    <t>D2 Centrifuge</t>
+  </si>
+  <si>
+    <t>12m/16</t>
+  </si>
+  <si>
+    <t>24m/12</t>
+  </si>
+  <si>
+    <t>WBIMultipurposeLab:CENTRIFUGE;PATH_HABITATION;PATH_SCIENCE</t>
+  </si>
+  <si>
+    <t>WBI_D2CryoShelter</t>
+  </si>
+  <si>
+    <t>D2 Cryo Shelter</t>
+  </si>
+  <si>
+    <t>f1.0/12</t>
+  </si>
+  <si>
+    <t>WBI_D2Greenhouse</t>
+  </si>
+  <si>
+    <t>D2 Greenhouse Module</t>
+  </si>
+  <si>
+    <t>Agroponics</t>
+  </si>
+  <si>
+    <t>WBI_D2Hab</t>
+  </si>
+  <si>
+    <t>D2 Habitat Module</t>
+  </si>
+  <si>
+    <t>WBIMultipurposeHab:D2HAB;PATH_HABITATION</t>
+  </si>
+  <si>
+    <t>12m/6</t>
+  </si>
+  <si>
+    <t>WBI_D2Office</t>
+  </si>
+  <si>
+    <t>D2 Briefing Room</t>
+  </si>
+  <si>
+    <t>f0.5/10</t>
+  </si>
+  <si>
+    <t>WBI_HomesteadMk3</t>
+  </si>
+  <si>
+    <t>Homestead Mk3</t>
+  </si>
+  <si>
+    <t>WBIMultipurposeLab:HOMESTEAD;PATH_HABITATION;PATH_SCIENCE;ROCKHOUND;PATH_INDUSTRY;STORAGE_TEMPLATE</t>
+  </si>
+  <si>
+    <t>wbiMeatLocker</t>
+  </si>
+  <si>
+    <t>Meat Locker CryoShelter</t>
+  </si>
+  <si>
+    <t>f1.0/4</t>
+  </si>
+  <si>
+    <t>quantumLeapAirlock</t>
+  </si>
+  <si>
+    <t>Quantum Leap Airlock</t>
+  </si>
+  <si>
+    <t>TranquilityHab</t>
+  </si>
+  <si>
+    <t>Tranquility Mk2 Habitat</t>
+  </si>
+  <si>
+    <t>WBIConvertibleMPL:TRANQ;PATH_HABITATION</t>
+  </si>
+  <si>
+    <t>wbiZenGreenhouse</t>
+  </si>
+  <si>
+    <t>Zen Mk2 Greenhouse</t>
+  </si>
+  <si>
+    <t>global construction module</t>
+  </si>
+  <si>
+    <t>wip</t>
+  </si>
+  <si>
+    <t>WBIMultipurposeLab:D2HAB;PATH_HABITATION;D2LAB;PATH_SCIENCE</t>
+  </si>
+  <si>
+    <t>50%/2</t>
   </si>
 </sst>
 </file>
@@ -301,7 +451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,8 +516,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +561,16 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -407,14 +581,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -438,12 +614,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,11 +917,12 @@
     <col min="6" max="6" width="12.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -824,7 +1005,9 @@
       <c r="M4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1104,6 +1287,9 @@
       <c r="M12" t="s">
         <v>33</v>
       </c>
+      <c r="N12" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1133,6 +1319,9 @@
       <c r="I13" t="s">
         <v>56</v>
       </c>
+      <c r="N13" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1165,6 +1354,9 @@
       <c r="J14" t="s">
         <v>55</v>
       </c>
+      <c r="N14" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1199,6 +1391,9 @@
       </c>
       <c r="M15" t="s">
         <v>33</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1221,7 +1416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1250,7 +1445,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1285,7 +1480,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1311,18 +1506,18 @@
         <v>75</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -1340,18 +1535,18 @@
         <v>45</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1369,18 +1564,18 @@
         <v>45</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1398,18 +1593,18 @@
         <v>45</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1427,7 +1622,468 @@
         <v>45</v>
       </c>
       <c r="J23" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="N26" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
+      <c r="F28" s="7">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="N28" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="14"/>
+      <c r="K30" t="s">
+        <v>103</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="G33" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="K37" t="s">
+        <v>138</v>
+      </c>
+      <c r="L37" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N37" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update partlist, pathfinder templates
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\ksp-mod-dev\WBIPlaymodeUSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B24451-9A15-4D6A-8F47-CF179C2021BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2234E837-8303-4D58-8106-1B1AC053A6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partlist" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="169">
   <si>
     <t>List of WBI parts and according USI configuration</t>
   </si>
@@ -463,6 +464,75 @@
   </si>
   <si>
     <t>Pathfinder</t>
+  </si>
+  <si>
+    <t>-template-</t>
+  </si>
+  <si>
+    <t>pigpen recycler</t>
+  </si>
+  <si>
+    <t>ponderosa hab</t>
+  </si>
+  <si>
+    <t>spyglass survey module</t>
+  </si>
+  <si>
+    <t>f0.25/1</t>
+  </si>
+  <si>
+    <t>PATH_HABITATION:Blacksmith</t>
+  </si>
+  <si>
+    <t>manufacturing</t>
+  </si>
+  <si>
+    <t>materiakits from ore -&gt;nerv!</t>
+  </si>
+  <si>
+    <t>PATH_INDUSTRY:Clockworks</t>
+  </si>
+  <si>
+    <t>PATH_INDUSTRY:Ironworks</t>
+  </si>
+  <si>
+    <t>lifesuport part</t>
+  </si>
+  <si>
+    <t>habitation pat</t>
+  </si>
+  <si>
+    <t>lifesupport (greenhouse)</t>
+  </si>
+  <si>
+    <t>ominconverter haber process</t>
+  </si>
+  <si>
+    <t>fertilizer from minerals</t>
+  </si>
+  <si>
+    <t>materialkits</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>polymer</t>
+  </si>
+  <si>
+    <t>chemical</t>
+  </si>
+  <si>
+    <t>metallicore</t>
+  </si>
+  <si>
+    <t>substrate</t>
+  </si>
+  <si>
+    <t>chemicals</t>
+  </si>
+  <si>
+    <t>minerals</t>
   </si>
 </sst>
 </file>
@@ -598,7 +668,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -623,6 +693,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -910,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,44 +2229,243 @@
       <c r="A42" t="s">
         <v>145</v>
       </c>
+      <c r="B42" t="s">
+        <v>149</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J42" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>145</v>
       </c>
+      <c r="B43" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G43" t="s">
+        <v>144</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I43" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>145</v>
       </c>
+      <c r="B44" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G44" t="s">
+        <v>147</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I44" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>145</v>
       </c>
+      <c r="B45" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G45" t="s">
+        <v>148</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I45" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>145</v>
       </c>
+      <c r="B46" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G46" t="s">
+        <v>151</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" t="s">
+        <v>152</v>
+      </c>
+      <c r="L46" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>145</v>
       </c>
+      <c r="B47" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G47" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I47" t="s">
+        <v>152</v>
+      </c>
+      <c r="L47" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" t="s">
+        <v>155</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" t="s">
+        <v>152</v>
+      </c>
+      <c r="L48" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>145</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G49" t="s">
+        <v>159</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" t="s">
+        <v>152</v>
+      </c>
+      <c r="L49" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFC7464-D34D-48C9-9F97-FE2E6CA7A9E0}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2.5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>